<commit_message>
Lab data for formal and impact testing
</commit_message>
<xml_diff>
--- a/Lab_1_Structures/impact_test_data.xlsx
+++ b/Lab_1_Structures/impact_test_data.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Height (in)</t>
   </si>
   <si>
-    <t>Force (ft lbs)</t>
-  </si>
-  <si>
     <t>Specimen</t>
   </si>
   <si>
@@ -67,12 +64,40 @@
   </si>
   <si>
     <t>Charpy</t>
+  </si>
+  <si>
+    <t>SHARPE (cm^2)</t>
+  </si>
+  <si>
+    <t>IZOD (cm^2)</t>
+  </si>
+  <si>
+    <t>Specimen Volume</t>
+  </si>
+  <si>
+    <t>IZOD (cm^3)</t>
+  </si>
+  <si>
+    <t>SHARPE (cm^3)</t>
+  </si>
+  <si>
+    <t>Specimen Corss-Sectional Area</t>
+  </si>
+  <si>
+    <t>Work (ft lbs)</t>
+  </si>
+  <si>
+    <t>Work Per Unit Volume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -90,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -113,25 +138,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,267 +467,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
+        <f>6.5-J10</f>
+        <v>12</v>
+      </c>
+      <c r="E2" s="9">
+        <f>D2/$L$4</f>
+        <v>40945.148675265824</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <f>4-$J$10</f>
+        <v>9.5</v>
+      </c>
+      <c r="E3" s="9">
+        <f t="shared" ref="E3:E7" si="0">D3/$L$4</f>
+        <v>32414.909367918779</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>7.4</v>
+      </c>
+      <c r="J3">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="K3">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <f>7-J10</f>
+        <v>12.5</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>42651.196536735231</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="6">
+        <f>I3*0.0328084</f>
+        <v>0.24278216000000002</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" ref="J4:K4" si="1">J3*0.0328084</f>
+        <v>3.4744095599999997E-2</v>
+      </c>
+      <c r="K4" s="6">
+        <f t="shared" si="1"/>
+        <v>3.4744095599999997E-2</v>
+      </c>
+      <c r="L4">
+        <f>I4*J4*K4</f>
+        <v>2.9307501348136436E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
+        <f>-1.5-J10</f>
+        <v>4</v>
+      </c>
+      <c r="E5" s="9">
+        <f t="shared" si="0"/>
+        <v>13648.382891755275</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2">
+        <f>59-$J$10</f>
+        <v>64.5</v>
+      </c>
+      <c r="E6" s="9">
+        <f t="shared" si="0"/>
+        <v>220080.17412955381</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>5.55</v>
+      </c>
+      <c r="J6">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="K6">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="L6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <f>58-J10</f>
+        <v>63.5</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>216668.07840661501</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="6">
+        <f>I6*0.0328084</f>
+        <v>0.18208662</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" ref="J7:K7" si="2">J6*0.0328084</f>
+        <v>3.4744095599999997E-2</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="2"/>
+        <v>3.4744095599999997E-2</v>
+      </c>
+      <c r="L7">
+        <f>I7*J7*K7</f>
+        <v>2.1980626011102329E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="4">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <f>18.75-I10</f>
+        <v>15.5</v>
+      </c>
+      <c r="E10" s="9">
+        <f>D10/$L$7</f>
+        <v>70516.644940735583</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="I10">
+        <v>3.25</v>
+      </c>
+      <c r="J10">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4">
-        <f>6.5-H10</f>
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
+        <f>17-I10</f>
+        <v>13.75</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" ref="E11:E15" si="3">D11/$L$7</f>
+        <v>62555.088253878341</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <f>14-I10</f>
+        <v>10.75</v>
+      </c>
+      <c r="E12" s="9">
+        <f t="shared" si="3"/>
+        <v>48906.705362123066</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="4">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="5"/>
-      <c r="B3" s="4" t="s">
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
+        <f>6.5-I10</f>
+        <v>3.25</v>
+      </c>
+      <c r="E13" s="9">
+        <f t="shared" si="3"/>
+        <v>14785.748132734881</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
+        <f>28.75-I10</f>
+        <v>25.5</v>
+      </c>
+      <c r="E14" s="9">
+        <f t="shared" si="3"/>
+        <v>116011.25457991983</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4">
-        <f>4-$H$10</f>
-        <v>9.5</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>7.4</v>
-      </c>
-      <c r="H3">
-        <v>1.0589999999999999</v>
-      </c>
-      <c r="I3">
-        <v>1.0589999999999999</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4">
-        <f>7-H10</f>
-        <v>12.5</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4">
-        <f>-1.5-H10</f>
-        <v>4</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
-        <f>59-$H$10</f>
-        <v>64.5</v>
-      </c>
-      <c r="F6" s="2">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>5.55</v>
-      </c>
-      <c r="H6">
-        <v>1.0589999999999999</v>
-      </c>
-      <c r="I6">
-        <v>1.0589999999999999</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4">
-        <f>58-H10</f>
-        <v>63.5</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="3"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
+        <f>29.875-I10</f>
+        <v>26.625</v>
+      </c>
+      <c r="E15" s="9">
+        <f t="shared" si="3"/>
+        <v>121129.39816432806</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="17" spans="4:11">
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="4:11">
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="7">
+        <f>I3*J3*K3</f>
+        <v>8.2989593999999993</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6">
+        <f>E18*0.393701^3</f>
+        <v>0.50643439510100696</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="7">
+        <f>I3*J3</f>
+        <v>7.8365999999999998</v>
+      </c>
+      <c r="K18" s="7">
+        <f>J18*0.393701^2</f>
+        <v>1.2146767412006767</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11">
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="7">
+        <f>I6*J6*K6</f>
+        <v>6.224219549999999</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6">
+        <f>E19*0.393701^3</f>
+        <v>0.37982579632575519</v>
+      </c>
+      <c r="I19" t="s">
         <v>16</v>
       </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="5">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
-        <f>18.75-G10</f>
-        <v>15.5</v>
-      </c>
-      <c r="G10">
-        <v>3.25</v>
-      </c>
-      <c r="H10">
-        <v>-5.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4">
-        <f>17-G10</f>
-        <v>13.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4">
-        <f>14-G10</f>
-        <v>10.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="5">
-        <v>2</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4">
-        <f>6.5-G10</f>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
-        <f>28.75-G10</f>
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4">
-        <f>29.875-G10</f>
-        <v>26.625</v>
+      <c r="J19" s="7">
+        <f>I6*J6</f>
+        <v>5.8774499999999996</v>
+      </c>
+      <c r="K19" s="7">
+        <f>J19*0.393701^2</f>
+        <v>0.91100755590050742</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="F6:F8"/>
+  <mergeCells count="8">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="H6:H8"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F3:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>